<commit_message>
Added/Update for Tick data
</commit_message>
<xml_diff>
--- a/data/raw_data/tick_survival_assay/TickSurvivalVeg_data_entry.xlsx
+++ b/data/raw_data/tick_survival_assay/TickSurvivalVeg_data_entry.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elena\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8774C1EB-0608-4EF7-8B54-052EE5EB1C23}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="45320" windowHeight="13800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="50">
   <si>
     <t>woody_veg_ht1</t>
   </si>
@@ -160,19 +159,22 @@
     <t>NA</t>
   </si>
   <si>
-    <t>missing</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
     <t xml:space="preserve">Y </t>
+  </si>
+  <si>
+    <t>Stem Density</t>
+  </si>
+  <si>
+    <t>Litter Cover</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -218,19 +220,72 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -567,14 +622,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AH28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB12" sqref="AB12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -582,7 +637,7 @@
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -644,7 +699,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -652,7 +707,7 @@
         <v>3161</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
         <v>44</v>
@@ -702,11 +757,20 @@
       <c r="S2">
         <v>0</v>
       </c>
-      <c r="T2">
-        <v>43.68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T2" s="2">
+        <v>48.879999999999995</v>
+      </c>
+      <c r="V2">
+        <f>AVERAGE(G2:I2)</f>
+        <v>106.33333333333333</v>
+      </c>
+      <c r="Y2" s="2">
+        <f>AVERAGE(J2:L2)</f>
+        <v>15.333333333333334</v>
+      </c>
+      <c r="Z2" s="2"/>
+    </row>
+    <row r="3" spans="1:34">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -714,7 +778,7 @@
         <v>3147</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
         <v>44</v>
@@ -764,11 +828,20 @@
       <c r="S3">
         <v>0</v>
       </c>
-      <c r="T3">
-        <v>72.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T3" s="2">
+        <v>51.480000000000004</v>
+      </c>
+      <c r="V3" s="2">
+        <f t="shared" ref="V3:V25" si="0">AVERAGE(G3:I3)</f>
+        <v>94.333333333333329</v>
+      </c>
+      <c r="Y3" s="2">
+        <f t="shared" ref="Y3:Y25" si="1">AVERAGE(J3:L3)</f>
+        <v>25.333333333333332</v>
+      </c>
+      <c r="Z3" s="2"/>
+    </row>
+    <row r="4" spans="1:34">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -776,7 +849,7 @@
         <v>3144</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
         <v>44</v>
@@ -826,11 +899,20 @@
       <c r="S4">
         <v>2</v>
       </c>
-      <c r="T4">
-        <v>53.04</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T4" s="2">
+        <v>48.620000000000005</v>
+      </c>
+      <c r="V4" s="2">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="Y4" s="2">
+        <f t="shared" si="1"/>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="Z4" s="2"/>
+    </row>
+    <row r="5" spans="1:34">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -838,7 +920,7 @@
         <v>3156</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
         <v>44</v>
@@ -888,11 +970,20 @@
       <c r="S5">
         <v>6</v>
       </c>
-      <c r="T5">
-        <v>63.44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T5" s="2">
+        <v>49.14</v>
+      </c>
+      <c r="V5" s="2">
+        <f t="shared" si="0"/>
+        <v>122.66666666666667</v>
+      </c>
+      <c r="Y5" s="2">
+        <f t="shared" si="1"/>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Z5" s="2"/>
+    </row>
+    <row r="6" spans="1:34">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -900,7 +991,7 @@
         <v>3154</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
         <v>44</v>
@@ -950,11 +1041,20 @@
       <c r="S6">
         <v>2</v>
       </c>
-      <c r="T6">
-        <v>31.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T6" s="2">
+        <v>50.18</v>
+      </c>
+      <c r="V6" s="2">
+        <f t="shared" si="0"/>
+        <v>92.666666666666671</v>
+      </c>
+      <c r="Y6" s="2">
+        <f t="shared" si="1"/>
+        <v>19.666666666666668</v>
+      </c>
+      <c r="Z6" s="2"/>
+    </row>
+    <row r="7" spans="1:34">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -962,7 +1062,7 @@
         <v>3143</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
         <v>44</v>
@@ -1012,11 +1112,20 @@
       <c r="S7">
         <v>2</v>
       </c>
-      <c r="T7">
-        <v>35.36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T7" s="2">
+        <v>48.36</v>
+      </c>
+      <c r="V7" s="2">
+        <f t="shared" si="0"/>
+        <v>121.66666666666667</v>
+      </c>
+      <c r="Y7" s="2">
+        <f t="shared" si="1"/>
+        <v>15.333333333333334</v>
+      </c>
+      <c r="Z7" s="2"/>
+    </row>
+    <row r="8" spans="1:34">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1024,7 +1133,7 @@
         <v>3146</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
         <v>44</v>
@@ -1074,11 +1183,20 @@
       <c r="S8">
         <v>0</v>
       </c>
-      <c r="T8">
-        <v>33.28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T8" s="2">
+        <v>42.379999999999995</v>
+      </c>
+      <c r="V8" s="2">
+        <f t="shared" si="0"/>
+        <v>95.333333333333329</v>
+      </c>
+      <c r="Y8" s="2">
+        <f t="shared" si="1"/>
+        <v>15.333333333333334</v>
+      </c>
+      <c r="Z8" s="2"/>
+    </row>
+    <row r="9" spans="1:34">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1086,7 +1204,7 @@
         <v>3151</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
         <v>44</v>
@@ -1133,14 +1251,23 @@
       <c r="R9">
         <v>48</v>
       </c>
-      <c r="S9" t="s">
-        <v>46</v>
-      </c>
-      <c r="T9">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9" s="2">
+        <v>56.16</v>
+      </c>
+      <c r="V9" s="2">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+      <c r="Y9" s="2">
+        <f t="shared" si="1"/>
+        <v>12.333333333333334</v>
+      </c>
+      <c r="Z9" s="2"/>
+    </row>
+    <row r="10" spans="1:34">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1148,7 +1275,7 @@
         <v>3153</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
         <v>44</v>
@@ -1198,11 +1325,20 @@
       <c r="S10">
         <v>0</v>
       </c>
-      <c r="T10">
-        <v>72.8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T10" s="2">
+        <v>58.24</v>
+      </c>
+      <c r="V10" s="2">
+        <f t="shared" si="0"/>
+        <v>104.66666666666667</v>
+      </c>
+      <c r="Y10" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="Z10" s="2"/>
+    </row>
+    <row r="11" spans="1:34">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1210,7 +1346,7 @@
         <v>3145</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11">
         <v>87</v>
@@ -1260,11 +1396,26 @@
       <c r="S11">
         <v>0</v>
       </c>
-      <c r="T11">
-        <v>80.08</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T11" s="2">
+        <v>44.720000000000006</v>
+      </c>
+      <c r="V11" s="2">
+        <f t="shared" si="0"/>
+        <v>117.33333333333333</v>
+      </c>
+      <c r="Y11" s="2">
+        <f t="shared" si="1"/>
+        <v>15.333333333333334</v>
+      </c>
+      <c r="Z11" s="2"/>
+      <c r="AB11" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1272,7 +1423,7 @@
         <v>3132</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
         <v>44</v>
@@ -1322,11 +1473,20 @@
       <c r="S12">
         <v>0</v>
       </c>
-      <c r="T12">
-        <v>82.16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T12" s="2">
+        <v>36.92</v>
+      </c>
+      <c r="V12" s="2">
+        <f t="shared" si="0"/>
+        <v>134.66666666666666</v>
+      </c>
+      <c r="Y12" s="2">
+        <f t="shared" si="1"/>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="Z12" s="2"/>
+    </row>
+    <row r="13" spans="1:34">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1334,7 +1494,7 @@
         <v>3148</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
         <v>44</v>
@@ -1384,11 +1544,51 @@
       <c r="S13">
         <v>0</v>
       </c>
-      <c r="T13">
-        <v>95.68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T13" s="2">
+        <v>44.2</v>
+      </c>
+      <c r="V13" s="2">
+        <f t="shared" si="0"/>
+        <v>103.66666666666667</v>
+      </c>
+      <c r="W13">
+        <f>AVERAGE(V2:V13)</f>
+        <v>112.19444444444446</v>
+      </c>
+      <c r="Y13" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Z13" s="2">
+        <f>AVERAGE(Y2:Y13)</f>
+        <v>14</v>
+      </c>
+      <c r="AB13">
+        <f>AVERAGE(P2:P13)</f>
+        <v>10.583333333333334</v>
+      </c>
+      <c r="AC13">
+        <f>STDEV(P2:P13)</f>
+        <v>9.5580364409255427</v>
+      </c>
+      <c r="AD13">
+        <f>AC13/SQRT(12)</f>
+        <v>2.7591674560463075</v>
+      </c>
+      <c r="AF13" s="2">
+        <f>AVERAGE(R2:R13)</f>
+        <v>35.666666666666664</v>
+      </c>
+      <c r="AG13" s="2">
+        <f>STDEV(R2:R13)</f>
+        <v>18.137521797911006</v>
+      </c>
+      <c r="AH13" s="2">
+        <f>AG13/SQRT(12)</f>
+        <v>5.2358515462283126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34">
       <c r="A14" s="2" t="s">
         <v>32</v>
       </c>
@@ -1396,7 +1596,7 @@
         <v>3165</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" s="2">
         <v>41</v>
@@ -1446,11 +1646,23 @@
       <c r="S14" s="2">
         <v>0</v>
       </c>
-      <c r="T14" s="2">
-        <v>93.6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T14" s="3">
+        <v>50.44</v>
+      </c>
+      <c r="V14" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="Y14" s="2">
+        <f t="shared" si="1"/>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="Z14" s="2"/>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="2"/>
+      <c r="AH14" s="2"/>
+    </row>
+    <row r="15" spans="1:34">
       <c r="A15" s="2" t="s">
         <v>33</v>
       </c>
@@ -1458,7 +1670,7 @@
         <v>3159</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" s="2">
         <v>20</v>
@@ -1508,11 +1720,23 @@
       <c r="S15" s="2">
         <v>0</v>
       </c>
-      <c r="T15" s="2">
-        <v>94.64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T15" s="3">
+        <v>52.52</v>
+      </c>
+      <c r="V15" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="Y15" s="2">
+        <f t="shared" si="1"/>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="Z15" s="2"/>
+      <c r="AF15" s="2"/>
+      <c r="AG15" s="2"/>
+      <c r="AH15" s="2"/>
+    </row>
+    <row r="16" spans="1:34">
       <c r="A16" s="2" t="s">
         <v>34</v>
       </c>
@@ -1520,7 +1744,7 @@
         <v>3166</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D16" s="2">
         <v>47</v>
@@ -1570,11 +1794,23 @@
       <c r="S16" s="2">
         <v>0</v>
       </c>
-      <c r="T16" s="2">
-        <v>88.4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T16" s="3">
+        <v>55.64</v>
+      </c>
+      <c r="V16" s="2">
+        <f t="shared" si="0"/>
+        <v>37.666666666666664</v>
+      </c>
+      <c r="Y16" s="2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="Z16" s="2"/>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="2"/>
+      <c r="AH16" s="2"/>
+    </row>
+    <row r="17" spans="1:34">
       <c r="A17" s="2" t="s">
         <v>35</v>
       </c>
@@ -1582,7 +1818,7 @@
         <v>3149</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D17" s="2">
         <v>176</v>
@@ -1632,11 +1868,23 @@
       <c r="S17" s="2">
         <v>0</v>
       </c>
-      <c r="T17" s="2">
-        <v>86.32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T17" s="3">
+        <v>45.5</v>
+      </c>
+      <c r="V17" s="2">
+        <f t="shared" si="0"/>
+        <v>22.333333333333332</v>
+      </c>
+      <c r="Y17" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Z17" s="2"/>
+      <c r="AF17" s="2"/>
+      <c r="AG17" s="2"/>
+      <c r="AH17" s="2"/>
+    </row>
+    <row r="18" spans="1:34">
       <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
@@ -1644,7 +1892,7 @@
         <v>3162</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" s="2">
         <v>66</v>
@@ -1694,11 +1942,23 @@
       <c r="S18" s="2">
         <v>0</v>
       </c>
-      <c r="T18" s="2">
-        <v>92.56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T18" s="3">
+        <v>50.96</v>
+      </c>
+      <c r="V18" s="2">
+        <f t="shared" si="0"/>
+        <v>44.666666666666664</v>
+      </c>
+      <c r="Y18" s="2">
+        <f t="shared" si="1"/>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="Z18" s="2"/>
+      <c r="AF18" s="2"/>
+      <c r="AG18" s="2"/>
+      <c r="AH18" s="2"/>
+    </row>
+    <row r="19" spans="1:34">
       <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
@@ -1706,7 +1966,7 @@
         <v>3155</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="2">
         <v>51</v>
@@ -1756,11 +2016,23 @@
       <c r="S19" s="2">
         <v>0</v>
       </c>
-      <c r="T19" s="2">
-        <v>94.64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T19" s="3">
+        <v>51.22</v>
+      </c>
+      <c r="V19" s="2">
+        <f t="shared" si="0"/>
+        <v>50.333333333333336</v>
+      </c>
+      <c r="Y19" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="Z19" s="2"/>
+      <c r="AF19" s="2"/>
+      <c r="AG19" s="2"/>
+      <c r="AH19" s="2"/>
+    </row>
+    <row r="20" spans="1:34">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
@@ -1768,7 +2040,7 @@
         <v>3157</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" s="2">
         <v>19</v>
@@ -1818,11 +2090,23 @@
       <c r="S20" s="2">
         <v>0</v>
       </c>
-      <c r="T20" s="2">
-        <v>87.36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T20" s="3">
+        <v>51.220000000000006</v>
+      </c>
+      <c r="V20" s="2">
+        <f t="shared" si="0"/>
+        <v>30.666666666666668</v>
+      </c>
+      <c r="Y20" s="2">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="Z20" s="2"/>
+      <c r="AF20" s="2"/>
+      <c r="AG20" s="2"/>
+      <c r="AH20" s="2"/>
+    </row>
+    <row r="21" spans="1:34">
       <c r="A21" s="2" t="s">
         <v>39</v>
       </c>
@@ -1830,7 +2114,7 @@
         <v>3160</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D21" s="2">
         <v>35</v>
@@ -1880,11 +2164,23 @@
       <c r="S21" s="2">
         <v>0</v>
       </c>
-      <c r="T21" s="2">
-        <v>88.4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T21" s="3">
+        <v>48.620000000000005</v>
+      </c>
+      <c r="V21" s="2">
+        <f t="shared" si="0"/>
+        <v>31.333333333333332</v>
+      </c>
+      <c r="Y21" s="2">
+        <f t="shared" si="1"/>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="Z21" s="2"/>
+      <c r="AF21" s="2"/>
+      <c r="AG21" s="2"/>
+      <c r="AH21" s="2"/>
+    </row>
+    <row r="22" spans="1:34">
       <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
@@ -1892,7 +2188,7 @@
         <v>3163</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D22" s="2">
         <v>100</v>
@@ -1942,11 +2238,23 @@
       <c r="S22" s="2">
         <v>0</v>
       </c>
-      <c r="T22" s="2">
-        <v>90.48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T22" s="3">
+        <v>44.980000000000004</v>
+      </c>
+      <c r="V22" s="2">
+        <f t="shared" si="0"/>
+        <v>37.666666666666664</v>
+      </c>
+      <c r="Y22" s="2">
+        <f t="shared" si="1"/>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="Z22" s="2"/>
+      <c r="AF22" s="2"/>
+      <c r="AG22" s="2"/>
+      <c r="AH22" s="2"/>
+    </row>
+    <row r="23" spans="1:34">
       <c r="A23" s="2" t="s">
         <v>41</v>
       </c>
@@ -1954,7 +2262,7 @@
         <v>3164</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>45</v>
@@ -2004,11 +2312,23 @@
       <c r="S23" s="2">
         <v>0</v>
       </c>
-      <c r="T23" s="2">
-        <v>92.56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T23" s="3">
+        <v>43.42</v>
+      </c>
+      <c r="V23" s="2">
+        <f t="shared" si="0"/>
+        <v>51.666666666666664</v>
+      </c>
+      <c r="Y23" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Z23" s="2"/>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2"/>
+      <c r="AH23" s="2"/>
+    </row>
+    <row r="24" spans="1:34">
       <c r="A24" s="2" t="s">
         <v>42</v>
       </c>
@@ -2016,7 +2336,7 @@
         <v>3150</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>45</v>
@@ -2066,11 +2386,23 @@
       <c r="S24" s="2">
         <v>0</v>
       </c>
-      <c r="T24" s="2">
-        <v>28.08</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T24" s="3">
+        <v>39.78</v>
+      </c>
+      <c r="V24" s="2">
+        <f t="shared" si="0"/>
+        <v>49.333333333333336</v>
+      </c>
+      <c r="Y24" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="Z24" s="2"/>
+      <c r="AF24" s="2"/>
+      <c r="AG24" s="2"/>
+      <c r="AH24" s="2"/>
+    </row>
+    <row r="25" spans="1:34">
       <c r="A25" s="2" t="s">
         <v>43</v>
       </c>
@@ -2078,7 +2410,7 @@
         <v>3158</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D25" s="2">
         <v>75</v>
@@ -2128,12 +2460,64 @@
       <c r="S25" s="2">
         <v>0</v>
       </c>
-      <c r="T25" s="2">
-        <v>35.36</v>
-      </c>
+      <c r="T25" s="3">
+        <v>33.800000000000004</v>
+      </c>
+      <c r="V25" s="2">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="W25" s="2">
+        <f>AVERAGE(V14:V25)</f>
+        <v>41.888888888888893</v>
+      </c>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2">
+        <f t="shared" si="1"/>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="Z25" s="2">
+        <f>AVERAGE(Y14:Y25)</f>
+        <v>4.416666666666667</v>
+      </c>
+      <c r="AB25" s="2">
+        <f>AVERAGE(P14:P25)</f>
+        <v>73.75</v>
+      </c>
+      <c r="AC25" s="2">
+        <f>STDEV(P14:P25)</f>
+        <v>22.373381099381959</v>
+      </c>
+      <c r="AD25" s="2">
+        <f>AC25/SQRT(12)</f>
+        <v>6.4586388002051303</v>
+      </c>
+      <c r="AF25" s="2">
+        <f>AVERAGE(R14:R25)</f>
+        <v>11.833333333333334</v>
+      </c>
+      <c r="AG25" s="2">
+        <f>STDEV(R14:R25)</f>
+        <v>4.7258156262526088</v>
+      </c>
+      <c r="AH25" s="2">
+        <f>AG25/SQRT(12)</f>
+        <v>1.3642254619787419</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34">
+      <c r="R27" s="2"/>
+    </row>
+    <row r="28" spans="1:34">
+      <c r="R28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>